<commit_message>
Añadido icono y título
</commit_message>
<xml_diff>
--- a/Documentación/Diseño/Controles_CartoonTrap.xlsx
+++ b/Documentación/Diseño/Controles_CartoonTrap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopth\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopth\github\CartoonTrap\Documentación\Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B229B81C-6D11-423A-8D40-FFD203031BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738F1947-EFB5-4804-8000-B74E344A384B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,48 +36,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
-    <t>Acción</t>
-  </si>
-  <si>
-    <t>Movimiento</t>
-  </si>
-  <si>
-    <t>Básico / Punch</t>
-  </si>
-  <si>
-    <t>Agarrar / Tirar</t>
-  </si>
-  <si>
     <t>Phiuu</t>
   </si>
   <si>
-    <t>Saltar / Hop</t>
-  </si>
-  <si>
-    <t>Espada / Slash</t>
-  </si>
-  <si>
-    <t>Martillo / Pum</t>
-  </si>
-  <si>
     <t>Dash</t>
   </si>
   <si>
-    <t>Ver mapa zona</t>
-  </si>
-  <si>
-    <t>Mapa completo</t>
-  </si>
-  <si>
-    <t>Pausa</t>
-  </si>
-  <si>
-    <t>Teclado Flechas</t>
-  </si>
-  <si>
-    <t>Mando (Xbox)</t>
-  </si>
-  <si>
     <t>Space</t>
   </si>
   <si>
@@ -129,15 +93,6 @@
     <t>Click Drch</t>
   </si>
   <si>
-    <t>Click Rueda Ratón</t>
-  </si>
-  <si>
-    <t>Teclado WASD sin ratón</t>
-  </si>
-  <si>
-    <t>Teclado WASD con ratón</t>
-  </si>
-  <si>
     <t>Left Joystick</t>
   </si>
   <si>
@@ -177,9 +132,6 @@
     <t>Escape</t>
   </si>
   <si>
-    <t>Cambiar configuración</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -196,6 +148,54 @@
   </si>
   <si>
     <t>Vídeo de como poner en funcionamiento Input System: https://www.youtube.com/watch?v=5tOOstXaIKE</t>
+  </si>
+  <si>
+    <t>Movement</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>Keyboard Arrows</t>
+  </si>
+  <si>
+    <t>Keyboard WASD without mouse</t>
+  </si>
+  <si>
+    <t>Keyboard WASD with mouse</t>
+  </si>
+  <si>
+    <t>Click Mouse Wheel</t>
+  </si>
+  <si>
+    <t>Basic Attack / Punch</t>
+  </si>
+  <si>
+    <t>Grap / Throw</t>
+  </si>
+  <si>
+    <t>Sword / Slash</t>
+  </si>
+  <si>
+    <t>Hammer / Pum</t>
+  </si>
+  <si>
+    <t>Jump / Hop</t>
+  </si>
+  <si>
+    <t>Zone map</t>
+  </si>
+  <si>
+    <t>Full zone</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>Change configuration</t>
   </si>
 </sst>
 </file>
@@ -699,258 +699,258 @@
   <dimension ref="B4:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="10" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>